<commit_message>
carga de graficos iniciales jans
</commit_message>
<xml_diff>
--- a/55_Entregable tabulados/insumos/Lista de tablas y figuras por realizar.xlsx
+++ b/55_Entregable tabulados/insumos/Lista de tablas y figuras por realizar.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA397F8-9D2E-4169-8DB7-A011D45953B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575FED99-5462-40E0-81A9-27BFBAEBC0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G15" sqref="A15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,25 +855,25 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="4" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>